<commit_message>
Update of morphometric parameters with addition of comparison between sources
</commit_message>
<xml_diff>
--- a/inputs/data/ALB_Morphometric_Parameters.xlsx
+++ b/inputs/data/ALB_Morphometric_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\Working_Parties\iotc-wptmt-data\inputs\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\repositories\data-analysis\MorphometricsALB\inputs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C3D212-0010-4B70-86EE-30D2D1376077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CA55CB-87D5-4792-9D1C-D762D50B4ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{13860A6C-8BD3-4438-8CDE-93AAFDA0ABAA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{13860A6C-8BD3-4438-8CDE-93AAFDA0ABAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="57">
   <si>
     <t>Area</t>
   </si>
@@ -175,6 +175,36 @@
   </si>
   <si>
     <t>LD1=a*FL+b</t>
+  </si>
+  <si>
+    <t>Working document</t>
+  </si>
+  <si>
+    <t>Kitakado et al (2019)</t>
+  </si>
+  <si>
+    <t>2012-2016</t>
+  </si>
+  <si>
+    <t>Huang1991</t>
+  </si>
+  <si>
+    <t>Hsu1999</t>
+  </si>
+  <si>
+    <t>Setyadji2012</t>
+  </si>
+  <si>
+    <t>Kitakado2019</t>
+  </si>
+  <si>
+    <t>Dhurmeea2016</t>
+  </si>
+  <si>
+    <t>Penney1994</t>
+  </si>
+  <si>
+    <t>ReferenceCode</t>
   </si>
 </sst>
 </file>
@@ -184,10 +214,17 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000E+00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -213,10 +250,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -235,9 +273,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -275,7 +313,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -381,7 +419,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -523,7 +561,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -531,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9734010B-4C15-4328-868D-55760F9011E3}">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,10 +588,11 @@
     <col min="13" max="13" width="12.140625" customWidth="1"/>
     <col min="14" max="14" width="10.85546875" customWidth="1"/>
     <col min="15" max="15" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.42578125" customWidth="1"/>
+    <col min="17" max="17" width="36.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -597,13 +636,16 @@
         <v>4</v>
       </c>
       <c r="O1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P1" t="s">
         <v>42</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -647,13 +689,16 @@
         <v>3.0973000000000002</v>
       </c>
       <c r="O2" t="s">
+        <v>55</v>
+      </c>
+      <c r="P2" t="s">
         <v>35</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -697,13 +742,16 @@
         <v>2.8570000000000002</v>
       </c>
       <c r="O3" t="s">
+        <v>50</v>
+      </c>
+      <c r="P3" t="s">
         <v>36</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -747,13 +795,16 @@
         <v>2.7513999999999998</v>
       </c>
       <c r="O4" t="s">
+        <v>51</v>
+      </c>
+      <c r="P4" t="s">
         <v>37</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -797,13 +848,16 @@
         <v>2.7271000000000001</v>
       </c>
       <c r="O5" t="s">
+        <v>52</v>
+      </c>
+      <c r="P5" t="s">
         <v>38</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -834,10 +888,10 @@
       <c r="J6">
         <v>118</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6">
         <v>5.4</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6">
         <v>33.1</v>
       </c>
       <c r="M6" s="1">
@@ -847,14 +901,17 @@
         <v>3.4239999999999999</v>
       </c>
       <c r="O6" t="s">
+        <v>54</v>
+      </c>
+      <c r="P6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>40</v>
       </c>
       <c r="C7" t="s">
@@ -881,10 +938,10 @@
       <c r="J7">
         <v>118</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7">
         <v>5.4</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7">
         <v>33.1</v>
       </c>
       <c r="M7">
@@ -894,10 +951,13 @@
         <v>0.61739999999999995</v>
       </c>
       <c r="O7" t="s">
+        <v>54</v>
+      </c>
+      <c r="P7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -928,10 +988,10 @@
       <c r="J8">
         <v>116</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8">
         <v>9.8000000000000007</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8">
         <v>31.3</v>
       </c>
       <c r="M8">
@@ -941,7 +1001,60 @@
         <v>5.4938000000000002</v>
       </c>
       <c r="O8" t="s">
+        <v>54</v>
+      </c>
+      <c r="P8" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9">
+        <v>8855</v>
+      </c>
+      <c r="I9">
+        <v>48</v>
+      </c>
+      <c r="J9">
+        <v>128</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9">
+        <v>35</v>
+      </c>
+      <c r="M9" s="2">
+        <v>6.8700999999999997E-6</v>
+      </c>
+      <c r="N9" s="3">
+        <v>3.2263999999999999</v>
+      </c>
+      <c r="O9" t="s">
+        <v>53</v>
+      </c>
+      <c r="P9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>